<commit_message>
Changed from prior training
</commit_message>
<xml_diff>
--- a/Mapping_Spreadsheets/niem-mapping-template.xlsx
+++ b/Mapping_Spreadsheets/niem-mapping-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10507"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-format-spreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcarlson31/Documents/NIEM-Training/Mapping_Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A9BE98-53A4-4BD4-B986-3E93087AB7CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC864DE7-0B81-4A40-AF8F-F755A739A47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10548" yWindow="1620" windowWidth="19440" windowHeight="11676" tabRatio="781" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="37220" windowHeight="21100" tabRatio="781" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" r:id="rId1"/>
@@ -4166,17 +4166,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" style="19" customWidth="1"/>
     <col min="2" max="2" width="51.33203125" style="19" customWidth="1"/>
     <col min="3" max="4" width="35" style="13" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="13"/>
+    <col min="5" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="90" t="s">
         <v>357</v>
       </c>
@@ -4184,21 +4186,21 @@
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>106</v>
       </c>
       <c r="B3" s="32"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="32"/>
       <c r="B4" s="32"/>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>94</v>
       </c>
@@ -4212,7 +4214,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
         <v>95</v>
       </c>
@@ -4226,7 +4228,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
         <v>118</v>
       </c>
@@ -4240,7 +4242,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="34" t="s">
         <v>109</v>
       </c>
@@ -4254,7 +4256,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="34" t="s">
         <v>110</v>
       </c>
@@ -4268,7 +4270,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="34" t="s">
         <v>113</v>
       </c>
@@ -4282,7 +4284,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="34" t="s">
         <v>97</v>
       </c>
@@ -4296,7 +4298,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="34" t="s">
         <v>98</v>
       </c>
@@ -4310,7 +4312,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
         <v>121</v>
       </c>
@@ -4324,15 +4326,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>99</v>
       </c>
@@ -4341,7 +4343,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="33" t="s">
         <v>92</v>
       </c>
@@ -4355,7 +4357,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
         <v>24</v>
       </c>
@@ -4369,7 +4371,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
         <v>25</v>
       </c>
@@ -4383,7 +4385,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
         <v>26</v>
       </c>
@@ -4397,7 +4399,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
         <v>27</v>
       </c>
@@ -4411,7 +4413,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="35" t="s">
         <v>41</v>
       </c>
@@ -4425,7 +4427,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="35" t="s">
         <v>42</v>
       </c>
@@ -4439,7 +4441,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="35" t="s">
         <v>298</v>
       </c>
@@ -4453,7 +4455,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="35" t="s">
         <v>43</v>
       </c>
@@ -4467,7 +4469,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A27" s="35" t="s">
         <v>208</v>
       </c>
@@ -4481,7 +4483,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="35" t="s">
         <v>267</v>
       </c>
@@ -4495,7 +4497,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
         <v>32</v>
       </c>
@@ -4503,7 +4505,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>33</v>
       </c>
@@ -4511,7 +4513,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>128</v>
       </c>
@@ -4519,7 +4521,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>34</v>
       </c>
@@ -4527,7 +4529,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>35</v>
       </c>
@@ -4535,7 +4537,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>37</v>
       </c>
@@ -4543,7 +4545,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>38</v>
       </c>
@@ -4551,7 +4553,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>40</v>
       </c>
@@ -4559,7 +4561,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="112" x14ac:dyDescent="0.2">
       <c r="A39" s="49" t="s">
         <v>250</v>
       </c>
@@ -4567,7 +4569,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A40" s="49" t="s">
         <v>254</v>
       </c>
@@ -4589,32 +4591,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:C204"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="18" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" style="19" customWidth="1"/>
     <col min="3" max="3" width="76" style="19" customWidth="1"/>
     <col min="4" max="5" width="29.33203125" style="18" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="18"/>
+    <col min="6" max="16384" width="8.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="75" t="s">
         <v>259</v>
       </c>
       <c r="B3" s="75"/>
       <c r="C3" s="75"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
         <v>261</v>
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="76"/>
       <c r="B5" s="77" t="s">
         <v>51</v>
@@ -4623,7 +4625,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="76"/>
       <c r="B6" s="77" t="s">
         <v>219</v>
@@ -4632,7 +4634,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="76"/>
       <c r="B7" s="77" t="s">
         <v>220</v>
@@ -4641,7 +4643,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="76"/>
       <c r="B8" s="77" t="s">
         <v>50</v>
@@ -4650,7 +4652,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="76"/>
       <c r="B9" s="77" t="s">
         <v>56</v>
@@ -4659,7 +4661,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="76"/>
       <c r="B10" s="77" t="s">
         <v>57</v>
@@ -4668,7 +4670,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="76"/>
       <c r="B11" s="77" t="s">
         <v>55</v>
@@ -4677,14 +4679,14 @@
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="56" t="s">
         <v>133</v>
       </c>
       <c r="B12" s="56"/>
       <c r="C12" s="56"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="76"/>
       <c r="B13" s="77" t="s">
         <v>60</v>
@@ -4693,14 +4695,14 @@
         <v>284</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="76"/>
       <c r="B14" s="77" t="s">
         <v>260</v>
       </c>
       <c r="C14" s="37"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="76"/>
       <c r="B15" s="78" t="s">
         <v>263</v>
@@ -4709,7 +4711,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="76"/>
       <c r="B16" s="78" t="s">
         <v>264</v>
@@ -4718,7 +4720,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="76"/>
       <c r="B17" s="78" t="s">
         <v>266</v>
@@ -4727,7 +4729,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="76"/>
       <c r="B18" s="78" t="s">
         <v>265</v>
@@ -4736,7 +4738,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="76"/>
       <c r="B19" s="78" t="s">
         <v>268</v>
@@ -4745,7 +4747,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="76"/>
       <c r="B20" s="78" t="s">
         <v>267</v>
@@ -4754,7 +4756,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="76"/>
       <c r="B21" s="78" t="s">
         <v>270</v>
@@ -4763,14 +4765,14 @@
         <v>288</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="76"/>
       <c r="B22" s="78" t="s">
         <v>269</v>
       </c>
       <c r="C22" s="37"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="76"/>
       <c r="B23" s="77" t="s">
         <v>50</v>
@@ -4779,7 +4781,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="76"/>
       <c r="B24" s="77" t="s">
         <v>58</v>
@@ -4788,7 +4790,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="76"/>
       <c r="B25" s="77" t="s">
         <v>55</v>
@@ -4797,14 +4799,14 @@
         <v>291</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="45" t="s">
         <v>262</v>
       </c>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="76"/>
       <c r="B27" s="77" t="s">
         <v>59</v>
@@ -4813,7 +4815,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="76"/>
       <c r="B28" s="77" t="s">
         <v>50</v>
@@ -4822,7 +4824,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="76"/>
       <c r="B29" s="77" t="s">
         <v>96</v>
@@ -4831,7 +4833,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="76"/>
       <c r="B30" s="77" t="s">
         <v>56</v>
@@ -4840,7 +4842,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="76"/>
       <c r="B31" s="77" t="s">
         <v>57</v>
@@ -4849,7 +4851,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="76"/>
       <c r="B32" s="77" t="s">
         <v>55</v>
@@ -4858,25 +4860,25 @@
         <v>297</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="41" t="s">
         <v>3</v>
       </c>
       <c r="B35" s="41"/>
       <c r="C35" s="41"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="42" t="s">
         <v>132</v>
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="42"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="43"/>
       <c r="B37" s="36" t="s">
         <v>135</v>
@@ -4885,7 +4887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="43"/>
       <c r="B38" s="36" t="s">
         <v>10</v>
@@ -4894,7 +4896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="43"/>
       <c r="B39" s="36" t="s">
         <v>11</v>
@@ -4903,7 +4905,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="43"/>
       <c r="B40" s="36" t="s">
         <v>0</v>
@@ -4912,14 +4914,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="56" t="s">
         <v>133</v>
       </c>
       <c r="B41" s="56"/>
       <c r="C41" s="56"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="44"/>
       <c r="B42" s="37" t="s">
         <v>7</v>
@@ -4928,14 +4930,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="45" t="s">
         <v>134</v>
       </c>
       <c r="B43" s="45"/>
       <c r="C43" s="45"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="46"/>
       <c r="B44" s="36" t="s">
         <v>135</v>
@@ -4944,7 +4946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="46"/>
       <c r="B45" s="36" t="s">
         <v>10</v>
@@ -4953,7 +4955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="46"/>
       <c r="B46" s="36" t="s">
         <v>224</v>
@@ -4962,7 +4964,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="46"/>
       <c r="B47" s="36" t="s">
         <v>0</v>
@@ -4971,7 +4973,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" s="46"/>
       <c r="B48" s="36" t="s">
         <v>12</v>
@@ -4980,14 +4982,14 @@
         <v>253</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="46"/>
       <c r="B49" s="36" t="s">
         <v>141</v>
       </c>
       <c r="C49" s="47"/>
     </row>
-    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="46"/>
       <c r="B50" s="55" t="s">
         <v>44</v>
@@ -4996,7 +4998,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="46"/>
       <c r="B51" s="55" t="s">
         <v>308</v>
@@ -5005,7 +5007,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="46"/>
       <c r="B52" s="55" t="s">
         <v>45</v>
@@ -5014,7 +5016,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="46"/>
       <c r="B53" s="36" t="s">
         <v>29</v>
@@ -5023,7 +5025,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="46"/>
       <c r="B54" s="36" t="s">
         <v>30</v>
@@ -5032,7 +5034,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="46"/>
       <c r="B55" s="36" t="s">
         <v>31</v>
@@ -5041,14 +5043,14 @@
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="58" t="s">
         <v>191</v>
       </c>
       <c r="B56" s="58"/>
       <c r="C56" s="58"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="9"/>
       <c r="B57" s="8" t="s">
         <v>192</v>
@@ -5057,7 +5059,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="9"/>
       <c r="B58" s="8" t="s">
         <v>198</v>
@@ -5066,7 +5068,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="9"/>
       <c r="B59" s="8" t="s">
         <v>201</v>
@@ -5075,7 +5077,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="9"/>
       <c r="B60" s="8" t="s">
         <v>199</v>
@@ -5084,7 +5086,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="9"/>
       <c r="B61" s="8" t="s">
         <v>200</v>
@@ -5093,36 +5095,36 @@
         <v>351</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="48"/>
       <c r="B62" s="49"/>
       <c r="C62" s="49"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="48"/>
       <c r="B63" s="49"/>
       <c r="C63" s="49"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="48"/>
       <c r="B64" s="49"/>
       <c r="C64" s="49"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="50" t="s">
         <v>4</v>
       </c>
       <c r="B65" s="51"/>
       <c r="C65" s="52"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="42" t="s">
         <v>132</v>
       </c>
       <c r="B66" s="42"/>
       <c r="C66" s="42"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="43"/>
       <c r="B67" s="36" t="s">
         <v>13</v>
@@ -5131,7 +5133,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="43"/>
       <c r="B68" s="36" t="s">
         <v>14</v>
@@ -5140,7 +5142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="43"/>
       <c r="B69" s="36" t="s">
         <v>28</v>
@@ -5149,7 +5151,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="43"/>
       <c r="B70" s="36" t="s">
         <v>0</v>
@@ -5158,14 +5160,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="56" t="s">
         <v>133</v>
       </c>
       <c r="B71" s="56"/>
       <c r="C71" s="56"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="44"/>
       <c r="B72" s="37" t="s">
         <v>7</v>
@@ -5174,14 +5176,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="45" t="s">
         <v>134</v>
       </c>
       <c r="B73" s="45"/>
       <c r="C73" s="45"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="44"/>
       <c r="B74" s="36" t="s">
         <v>13</v>
@@ -5190,7 +5192,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="44"/>
       <c r="B75" s="36" t="s">
         <v>14</v>
@@ -5199,7 +5201,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="44"/>
       <c r="B76" s="36" t="s">
         <v>0</v>
@@ -5208,7 +5210,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="44"/>
       <c r="B77" s="36" t="s">
         <v>28</v>
@@ -5217,14 +5219,14 @@
         <v>162</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="44"/>
       <c r="B78" s="36" t="s">
         <v>46</v>
       </c>
       <c r="C78" s="36"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="44"/>
       <c r="B79" s="55" t="s">
         <v>300</v>
@@ -5233,7 +5235,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="44"/>
       <c r="B80" s="55" t="s">
         <v>301</v>
@@ -5242,7 +5244,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="44"/>
       <c r="B81" s="55" t="s">
         <v>302</v>
@@ -5251,7 +5253,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="44"/>
       <c r="B82" s="55" t="s">
         <v>303</v>
@@ -5260,7 +5262,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="44"/>
       <c r="B83" s="55" t="s">
         <v>304</v>
@@ -5269,7 +5271,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="44"/>
       <c r="B84" s="55" t="s">
         <v>143</v>
@@ -5278,7 +5280,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="44"/>
       <c r="B85" s="55" t="s">
         <v>305</v>
@@ -5287,7 +5289,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="44"/>
       <c r="B86" s="55" t="s">
         <v>306</v>
@@ -5296,7 +5298,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="44"/>
       <c r="B87" s="55" t="s">
         <v>307</v>
@@ -5305,7 +5307,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="44"/>
       <c r="B88" s="36" t="s">
         <v>328</v>
@@ -5314,7 +5316,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A89" s="44"/>
       <c r="B89" s="36" t="s">
         <v>353</v>
@@ -5323,7 +5325,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="44"/>
       <c r="B90" s="36" t="s">
         <v>329</v>
@@ -5332,14 +5334,14 @@
         <v>332</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="58" t="s">
         <v>191</v>
       </c>
       <c r="B91" s="58"/>
       <c r="C91" s="58"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="9"/>
       <c r="B92" s="8" t="s">
         <v>192</v>
@@ -5348,7 +5350,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="9"/>
       <c r="B93" s="8" t="s">
         <v>327</v>
@@ -5357,7 +5359,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="9"/>
       <c r="B94" s="8" t="s">
         <v>196</v>
@@ -5366,36 +5368,36 @@
         <v>352</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="48"/>
       <c r="B95" s="49"/>
       <c r="C95" s="49"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="48"/>
       <c r="B96" s="49"/>
       <c r="C96" s="49"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="48"/>
       <c r="B97" s="49"/>
       <c r="C97" s="49"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="50" t="s">
         <v>153</v>
       </c>
       <c r="B98" s="51"/>
       <c r="C98" s="52"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="42" t="s">
         <v>132</v>
       </c>
       <c r="B99" s="42"/>
       <c r="C99" s="42"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="43"/>
       <c r="B100" s="36" t="s">
         <v>154</v>
@@ -5404,7 +5406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="43"/>
       <c r="B101" s="36" t="s">
         <v>14</v>
@@ -5413,7 +5415,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="43"/>
       <c r="B102" s="36" t="s">
         <v>63</v>
@@ -5422,7 +5424,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="43"/>
       <c r="B103" s="36" t="s">
         <v>10</v>
@@ -5431,7 +5433,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="43"/>
       <c r="B104" s="36" t="s">
         <v>66</v>
@@ -5440,7 +5442,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="43"/>
       <c r="B105" s="36" t="s">
         <v>67</v>
@@ -5449,14 +5451,14 @@
         <v>158</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="56" t="s">
         <v>133</v>
       </c>
       <c r="B106" s="56"/>
       <c r="C106" s="56"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="44"/>
       <c r="B107" s="37" t="s">
         <v>7</v>
@@ -5465,14 +5467,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="45" t="s">
         <v>134</v>
       </c>
       <c r="B108" s="45"/>
       <c r="C108" s="45"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="43"/>
       <c r="B109" s="36" t="s">
         <v>154</v>
@@ -5481,7 +5483,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="43"/>
       <c r="B110" s="36" t="s">
         <v>14</v>
@@ -5490,7 +5492,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="43"/>
       <c r="B111" s="36" t="s">
         <v>63</v>
@@ -5499,7 +5501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="43"/>
       <c r="B112" s="36" t="s">
         <v>10</v>
@@ -5508,7 +5510,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="113" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="43"/>
       <c r="B113" s="36" t="s">
         <v>66</v>
@@ -5517,7 +5519,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="43"/>
       <c r="B114" s="55" t="s">
         <v>65</v>
@@ -5526,7 +5528,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="43"/>
       <c r="B115" s="36" t="s">
         <v>67</v>
@@ -5535,7 +5537,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="43"/>
       <c r="B116" s="55" t="s">
         <v>159</v>
@@ -5544,7 +5546,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="43"/>
       <c r="B117" s="36" t="s">
         <v>0</v>
@@ -5553,7 +5555,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="43"/>
       <c r="B118" s="36" t="s">
         <v>309</v>
@@ -5562,14 +5564,14 @@
         <v>310</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="58" t="s">
         <v>191</v>
       </c>
       <c r="B119" s="58"/>
       <c r="C119" s="58"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="9"/>
       <c r="B120" s="9" t="s">
         <v>192</v>
@@ -5578,26 +5580,26 @@
         <v>194</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="53"/>
       <c r="B121" s="54"/>
       <c r="C121" s="54"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="50" t="s">
         <v>299</v>
       </c>
       <c r="B124" s="51"/>
       <c r="C124" s="57"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="42" t="s">
         <v>132</v>
       </c>
       <c r="B125" s="42"/>
       <c r="C125" s="42"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="43"/>
       <c r="B126" s="36" t="s">
         <v>165</v>
@@ -5606,7 +5608,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="43"/>
       <c r="B127" s="36" t="s">
         <v>14</v>
@@ -5615,7 +5617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="43"/>
       <c r="B128" s="36" t="s">
         <v>71</v>
@@ -5624,7 +5626,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="43"/>
       <c r="B129" s="36" t="s">
         <v>0</v>
@@ -5633,14 +5635,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="56" t="s">
         <v>133</v>
       </c>
       <c r="B130" s="56"/>
       <c r="C130" s="56"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="44"/>
       <c r="B131" s="37" t="s">
         <v>7</v>
@@ -5649,14 +5651,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="45" t="s">
         <v>134</v>
       </c>
       <c r="B132" s="45"/>
       <c r="C132" s="45"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="43"/>
       <c r="B133" s="36" t="s">
         <v>165</v>
@@ -5665,7 +5667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="43"/>
       <c r="B134" s="36" t="s">
         <v>14</v>
@@ -5674,7 +5676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="44"/>
       <c r="B135" s="36" t="s">
         <v>71</v>
@@ -5683,7 +5685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="44"/>
       <c r="B136" s="36" t="s">
         <v>0</v>
@@ -5692,7 +5694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="44"/>
       <c r="B137" s="36" t="s">
         <v>1</v>
@@ -5701,7 +5703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="44"/>
       <c r="B138" s="55" t="s">
         <v>167</v>
@@ -5710,7 +5712,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="44"/>
       <c r="B139" s="55" t="s">
         <v>168</v>
@@ -5719,7 +5721,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="44"/>
       <c r="B140" s="55" t="s">
         <v>171</v>
@@ -5728,7 +5730,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="44"/>
       <c r="B141" s="55" t="s">
         <v>172</v>
@@ -5737,7 +5739,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="44"/>
       <c r="B142" s="55" t="s">
         <v>169</v>
@@ -5746,7 +5748,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="44"/>
       <c r="B143" s="55" t="s">
         <v>170</v>
@@ -5755,7 +5757,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="44"/>
       <c r="B144" s="55" t="s">
         <v>173</v>
@@ -5764,7 +5766,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="44"/>
       <c r="B145" s="55" t="s">
         <v>174</v>
@@ -5773,7 +5775,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="44"/>
       <c r="B146" s="55" t="s">
         <v>175</v>
@@ -5782,7 +5784,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="44"/>
       <c r="B147" s="55" t="s">
         <v>176</v>
@@ -5791,7 +5793,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="44"/>
       <c r="B148" s="55" t="s">
         <v>177</v>
@@ -5800,7 +5802,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="44"/>
       <c r="B149" s="55" t="s">
         <v>178</v>
@@ -5809,14 +5811,14 @@
         <v>190</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="58" t="s">
         <v>191</v>
       </c>
       <c r="B150" s="58"/>
       <c r="C150" s="58"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="9"/>
       <c r="B151" s="9" t="s">
         <v>192</v>
@@ -5825,36 +5827,36 @@
         <v>193</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="48"/>
       <c r="B152" s="49"/>
       <c r="C152" s="49"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="48"/>
       <c r="B153" s="49"/>
       <c r="C153" s="49"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="48"/>
       <c r="B154" s="49"/>
       <c r="C154" s="49"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="50" t="s">
         <v>5</v>
       </c>
       <c r="B155" s="51"/>
       <c r="C155" s="52"/>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="42" t="s">
         <v>132</v>
       </c>
       <c r="B156" s="42"/>
       <c r="C156" s="42"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="43"/>
       <c r="B157" s="36" t="s">
         <v>165</v>
@@ -5863,7 +5865,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="43"/>
       <c r="B158" s="36" t="s">
         <v>20</v>
@@ -5872,7 +5874,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="43"/>
       <c r="B159" s="36" t="s">
         <v>0</v>
@@ -5881,14 +5883,14 @@
         <v>206</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="56" t="s">
         <v>133</v>
       </c>
       <c r="B160" s="56"/>
       <c r="C160" s="56"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="44"/>
       <c r="B161" s="37" t="s">
         <v>7</v>
@@ -5897,14 +5899,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="45" t="s">
         <v>134</v>
       </c>
       <c r="B162" s="45"/>
       <c r="C162" s="45"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="44"/>
       <c r="B163" s="36" t="s">
         <v>165</v>
@@ -5913,14 +5915,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="44"/>
       <c r="B164" s="36" t="s">
         <v>46</v>
       </c>
       <c r="C164" s="36"/>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="44"/>
       <c r="B165" s="55" t="s">
         <v>334</v>
@@ -5929,7 +5931,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A166" s="44"/>
       <c r="B166" s="55" t="s">
         <v>335</v>
@@ -5938,7 +5940,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="44"/>
       <c r="B167" s="55" t="s">
         <v>336</v>
@@ -5947,7 +5949,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="44"/>
       <c r="B168" s="55" t="s">
         <v>337</v>
@@ -5956,7 +5958,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="44"/>
       <c r="B169" s="55" t="s">
         <v>301</v>
@@ -5965,7 +5967,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="44"/>
       <c r="B170" s="55" t="s">
         <v>343</v>
@@ -5974,7 +5976,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="44"/>
       <c r="B171" s="55" t="s">
         <v>345</v>
@@ -5983,7 +5985,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="44"/>
       <c r="B172" s="55" t="s">
         <v>338</v>
@@ -5992,7 +5994,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="44"/>
       <c r="B173" s="55" t="s">
         <v>339</v>
@@ -6001,7 +6003,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="44"/>
       <c r="B174" s="55" t="s">
         <v>340</v>
@@ -6010,7 +6012,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="44"/>
       <c r="B175" s="55" t="s">
         <v>342</v>
@@ -6019,7 +6021,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="44"/>
       <c r="B176" s="55" t="s">
         <v>341</v>
@@ -6028,7 +6030,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="44"/>
       <c r="B177" s="36" t="s">
         <v>20</v>
@@ -6037,7 +6039,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="44"/>
       <c r="B178" s="36" t="s">
         <v>0</v>
@@ -6046,7 +6048,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="44"/>
       <c r="B179" s="36" t="s">
         <v>241</v>
@@ -6055,7 +6057,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="44"/>
       <c r="B180" s="55" t="s">
         <v>240</v>
@@ -6064,7 +6066,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A181" s="44"/>
       <c r="B181" s="55" t="s">
         <v>239</v>
@@ -6073,7 +6075,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="44"/>
       <c r="B182" s="36" t="s">
         <v>225</v>
@@ -6082,7 +6084,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="44"/>
       <c r="B183" s="36" t="s">
         <v>226</v>
@@ -6091,7 +6093,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="44"/>
       <c r="B184" s="36" t="s">
         <v>205</v>
@@ -6100,14 +6102,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="58" t="s">
         <v>191</v>
       </c>
       <c r="B185" s="58"/>
       <c r="C185" s="58"/>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="9"/>
       <c r="B186" s="9" t="s">
         <v>192</v>
@@ -6116,21 +6118,21 @@
         <v>202</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="50" t="s">
         <v>319</v>
       </c>
       <c r="B190" s="51"/>
       <c r="C190" s="52"/>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="42" t="s">
         <v>132</v>
       </c>
       <c r="B191" s="42"/>
       <c r="C191" s="42"/>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="43"/>
       <c r="B192" s="36" t="s">
         <v>320</v>
@@ -6139,7 +6141,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="43"/>
       <c r="B193" s="36" t="s">
         <v>213</v>
@@ -6148,7 +6150,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="43"/>
       <c r="B194" s="36" t="s">
         <v>212</v>
@@ -6157,7 +6159,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="43"/>
       <c r="B195" s="36" t="s">
         <v>0</v>
@@ -6166,14 +6168,14 @@
         <v>216</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="56" t="s">
         <v>133</v>
       </c>
       <c r="B196" s="56"/>
       <c r="C196" s="56"/>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="44"/>
       <c r="B197" s="37" t="s">
         <v>7</v>
@@ -6182,14 +6184,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="45" t="s">
         <v>134</v>
       </c>
       <c r="B198" s="45"/>
       <c r="C198" s="45"/>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="44"/>
       <c r="B199" s="36" t="s">
         <v>320</v>
@@ -6198,7 +6200,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="44"/>
       <c r="B200" s="36" t="s">
         <v>213</v>
@@ -6207,7 +6209,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="44"/>
       <c r="B201" s="36" t="s">
         <v>212</v>
@@ -6216,7 +6218,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="44"/>
       <c r="B202" s="36" t="s">
         <v>0</v>
@@ -6225,14 +6227,14 @@
         <v>216</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" s="58" t="s">
         <v>191</v>
       </c>
       <c r="B203" s="58"/>
       <c r="C203" s="58"/>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="9"/>
       <c r="B204" s="9" t="s">
         <v>192</v>
@@ -6270,20 +6272,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="86.44140625" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="24.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="86.5" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="20"/>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>52</v>
       </c>
@@ -6291,57 +6293,57 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>219</v>
       </c>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>220</v>
       </c>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>55</v>
       </c>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="20"/>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
         <v>54</v>
       </c>
@@ -6349,45 +6351,45 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="74" t="s">
         <v>260</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>55</v>
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
         <v>53</v>
       </c>
@@ -6395,51 +6397,51 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
         <v>96</v>
       </c>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
         <v>55</v>
       </c>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="20"/>
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>61</v>
       </c>
@@ -6477,7 +6479,7 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
     <col min="2" max="3" width="29.6640625" style="2" customWidth="1"/>
@@ -6490,11 +6492,11 @@
     <col min="12" max="12" width="29.6640625" style="2" customWidth="1"/>
     <col min="13" max="13" width="17.33203125" style="2" customWidth="1"/>
     <col min="14" max="14" width="31.33203125" style="2" customWidth="1"/>
-    <col min="15" max="17" width="31.88671875" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="2"/>
+    <col min="15" max="17" width="31.83203125" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="62" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="62" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
@@ -6576,23 +6578,23 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
     <col min="2" max="3" width="29.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="45.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="22.33203125" style="2" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" style="2" customWidth="1"/>
     <col min="9" max="10" width="29.6640625" style="2" customWidth="1"/>
     <col min="11" max="11" width="45.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16.5546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="16.5" style="2" customWidth="1"/>
     <col min="13" max="14" width="45.6640625" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="2"/>
+    <col min="15" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="62" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="62" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
@@ -6668,28 +6670,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.6640625" style="2" customWidth="1"/>
     <col min="5" max="6" width="11.6640625" style="19" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="23.88671875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="23.83203125" style="2" customWidth="1"/>
     <col min="12" max="12" width="14" style="2" customWidth="1"/>
     <col min="13" max="13" width="30.6640625" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.6640625" style="19" customWidth="1"/>
-    <col min="15" max="15" width="14.44140625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="14.5" style="19" customWidth="1"/>
     <col min="16" max="16" width="43.6640625" style="2" customWidth="1"/>
     <col min="17" max="17" width="12.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="2"/>
+    <col min="18" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="62" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="62" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>62</v>
       </c>
@@ -6742,7 +6744,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="79"/>
       <c r="E2" s="81"/>
       <c r="F2" s="81"/>
@@ -6779,25 +6781,25 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="19" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" style="19" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="24.5" style="19" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="19" customWidth="1"/>
     <col min="7" max="7" width="20.33203125" style="19" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" style="19" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="19" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" style="19" customWidth="1"/>
-    <col min="10" max="10" width="32.88671875" style="19" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" style="19" customWidth="1"/>
+    <col min="10" max="10" width="32.83203125" style="19" customWidth="1"/>
+    <col min="11" max="11" width="17.5" style="19" customWidth="1"/>
     <col min="12" max="12" width="40.6640625" style="19" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" style="19" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="19"/>
+    <col min="13" max="13" width="22.1640625" style="19" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="63" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="63" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="67" t="s">
         <v>68</v>
       </c>
@@ -6838,7 +6840,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="66"/>
       <c r="B2" s="66"/>
       <c r="C2" s="66"/>
@@ -6887,26 +6889,26 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="55.6640625" style="64" customWidth="1"/>
     <col min="3" max="3" width="35.6640625" style="64" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
-    <col min="5" max="6" width="29.109375" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="29.1640625" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="23.6640625" style="64" customWidth="1"/>
     <col min="8" max="8" width="13" style="64" customWidth="1"/>
     <col min="9" max="9" width="55.6640625" style="64" customWidth="1"/>
     <col min="10" max="10" width="35.6640625" style="64" customWidth="1"/>
     <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="23.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="35.44140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="23.5" style="2" customWidth="1"/>
+    <col min="13" max="13" width="35.5" style="2" customWidth="1"/>
     <col min="14" max="14" width="23.6640625" style="65" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="2"/>
+    <col min="15" max="15" width="9.1640625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="62" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="62" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="88" t="s">
         <v>203</v>
       </c>
@@ -6985,21 +6987,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
-    <col min="2" max="4" width="20.5546875" style="2" customWidth="1"/>
+    <col min="2" max="4" width="20.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" style="19" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="19" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" style="19" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="23.88671875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="23.83203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="30.6640625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="2"/>
+    <col min="12" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>258</v>
       </c>
@@ -7034,7 +7036,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F2" s="66"/>
       <c r="G2" s="66"/>
     </row>

</xml_diff>